<commit_message>
Add all my files
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Downloads\marsframework-master\marsframework-master\MarsFramework\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\source\repos\marsframework-master\marsframework-master\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BE6ED8-EB5D-4A74-8948-1C063125DEBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790144CC-323B-47FA-8AF2-47DD4B74C1BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>Url</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>SydneyQa2018</t>
+  </si>
+  <si>
+    <t>SydneyQa2019</t>
   </si>
 </sst>
 </file>
@@ -578,10 +581,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,13 +616,22 @@
         <v>33</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{A602A4E5-4248-4793-895E-EEE275AB5752}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{3115C0C2-9D9A-4D61-9622-BDED313F4F26}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>